<commit_message>
Update with new survey dates
</commit_message>
<xml_diff>
--- a/data-raw/Site Metadata Git- 2017.xlsx
+++ b/data-raw/Site Metadata Git- 2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sethapp\Documents\Git Preliminary Work- Not Synced to R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sethapp\Documents\Git\ISUmonarch\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
@@ -973,7 +973,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>